<commit_message>
Updated UI section in SDD
</commit_message>
<xml_diff>
--- a/Task Delegation.xlsx
+++ b/Task Delegation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Magev\OneDrive\Desktop\Data Science\Tri 2 2023\SoftwareTech\AssignmentGit\2810ICT_Assignment_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\2810ICT_Assignment_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CBA01328-4D6C-4B15-9872-E76ABDBB9089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855E82ED-F5F4-4477-B254-D4AF4E3476E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{137F4D14-D38C-4D8D-9D39-C195F808DA97}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{137F4D14-D38C-4D8D-9D39-C195F808DA97}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Part A</t>
   </si>
@@ -102,7 +100,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,8 +136,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -211,6 +216,17 @@
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -223,7 +239,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -237,8 +253,9 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="12"/>
@@ -258,8 +275,10 @@
     <xf numFmtId="9" fontId="0" fillId="8" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="7" borderId="0" xfId="6" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="13"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="14">
     <cellStyle name="20% - Accent2" xfId="6" builtinId="34"/>
     <cellStyle name="40% - Accent2" xfId="7" builtinId="35"/>
     <cellStyle name="40% - Accent4" xfId="10" builtinId="43"/>
@@ -272,6 +291,7 @@
     <cellStyle name="Accent4" xfId="9" builtinId="41"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="13" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -586,7 +606,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA5E3295-B424-4A84-B5FF-24E1614E0F8C}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -604,8 +626,8 @@
         <v>15</v>
       </c>
       <c r="G2" s="1">
-        <f>B4+B5</f>
-        <v>0.15000000000000002</v>
+        <f>B4+B5+B15</f>
+        <v>0.30000000000000004</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -636,6 +658,10 @@
       <c r="F4" t="s">
         <v>17</v>
       </c>
+      <c r="G4" s="1">
+        <f>B10+B11</f>
+        <v>0.2</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -685,6 +711,9 @@
       <c r="B10" s="9">
         <v>0.1</v>
       </c>
+      <c r="C10" s="19" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
@@ -693,6 +722,9 @@
       <c r="B11" s="9">
         <v>0.1</v>
       </c>
+      <c r="C11" s="19" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
@@ -707,6 +739,7 @@
       <c r="B13" s="17">
         <v>0.05</v>
       </c>
+      <c r="C13" s="20"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
@@ -715,6 +748,7 @@
       <c r="B14" s="17">
         <v>0.1</v>
       </c>
+      <c r="C14" s="20"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
@@ -722,6 +756,9 @@
       </c>
       <c r="B15" s="16">
         <v>0.15</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>